<commit_message>
:pencil2: upload-certificate,  data schema: add studentId field
</commit_message>
<xml_diff>
--- a/public/static/excels/bang-cap-example.xlsx
+++ b/public/static/excels/bang-cap-example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\projects\b4e_new\school\frontend\public\static\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{357EEED6-EF8B-4443-A9BA-542048114AA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAC05B2-DF61-40FA-BC5B-03DA162D9823}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21630" yWindow="735" windowWidth="17280" windowHeight="9075" xr2:uid="{317A8C35-2594-415E-885E-BAAE4C8658CD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{317A8C35-2594-415E-885E-BAAE4C8658CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>Họ và tên</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Nguyễn Văn Bình</t>
+  </si>
+  <si>
+    <t>Mã số sinh viên</t>
   </si>
 </sst>
 </file>
@@ -461,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3669C15-3A26-4249-9803-5F1256BFC111}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:N3"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,7 +483,7 @@
     <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -523,8 +526,11 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -567,8 +573,11 @@
       <c r="N2">
         <v>12341231431</v>
       </c>
+      <c r="O2">
+        <v>20161234</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -610,6 +619,9 @@
       </c>
       <c r="N3">
         <v>1234123143</v>
+      </c>
+      <c r="O3">
+        <v>20161235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>